<commit_message>
update for first basic version
</commit_message>
<xml_diff>
--- a/output/example_schedule.xlsx
+++ b/output/example_schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Stunde</t>
   </si>
@@ -22,16 +22,19 @@
     <t>01.12.2021</t>
   </si>
   <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>44</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>43</t>
+    <t>17</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
   <si>
     <t>02.12.2021</t>
@@ -43,10 +46,10 @@
     <t>03.12.2021</t>
   </si>
   <si>
+    <t>18</t>
+  </si>
+  <si>
     <t>04.12.2021</t>
-  </si>
-  <si>
-    <t>20</t>
   </si>
 </sst>
 </file>
@@ -423,13 +426,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" customHeight="1">
@@ -437,7 +440,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14" customHeight="1">
@@ -445,7 +448,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14" customHeight="1">
@@ -502,10 +505,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14" customHeight="1">
@@ -513,10 +516,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14" customHeight="1">
@@ -524,10 +527,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14" customHeight="1">
@@ -543,7 +546,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14" customHeight="1">
@@ -576,7 +579,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14" customHeight="1">
@@ -584,7 +587,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14" customHeight="1">
@@ -592,7 +595,7 @@
         <v>22</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14" customHeight="1">
@@ -600,7 +603,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed minor bugs in SCSM and added evaluation script
</commit_message>
<xml_diff>
--- a/output/example_schedule.xlsx
+++ b/output/example_schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Stunde</t>
   </si>
@@ -25,31 +25,34 @@
     <t>22</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>21</t>
   </si>
   <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>02.12.2021</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>03.12.2021</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>04.12.2021</t>
+  </si>
+  <si>
     <t>44</t>
   </si>
   <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>02.12.2021</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>03.12.2021</t>
-  </si>
-  <si>
     <t>18</t>
-  </si>
-  <si>
-    <t>04.12.2021</t>
   </si>
 </sst>
 </file>
@@ -426,13 +429,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" customHeight="1">
@@ -440,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14" customHeight="1">
@@ -448,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14" customHeight="1">
@@ -505,10 +508,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14" customHeight="1">
@@ -516,7 +519,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
@@ -527,10 +530,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14" customHeight="1">
@@ -538,7 +541,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14" customHeight="1">
@@ -546,7 +549,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14" customHeight="1">
@@ -579,7 +582,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14" customHeight="1">
@@ -587,7 +590,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14" customHeight="1">
@@ -595,7 +598,7 @@
         <v>22</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14" customHeight="1">
@@ -603,7 +606,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved SCSM to read report data from sqlite database
</commit_message>
<xml_diff>
--- a/output/example_schedule.xlsx
+++ b/output/example_schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Stunde</t>
   </si>
@@ -22,37 +22,46 @@
     <t>01.12.2021</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>43</t>
+    <t>917</t>
+  </si>
+  <si>
+    <t>944</t>
+  </si>
+  <si>
+    <t>943</t>
+  </si>
+  <si>
+    <t>722</t>
+  </si>
+  <si>
+    <t>922</t>
+  </si>
+  <si>
+    <t>701</t>
   </si>
   <si>
     <t>02.12.2021</t>
   </si>
   <si>
-    <t>17</t>
+    <t>151</t>
+  </si>
+  <si>
+    <t>720</t>
   </si>
   <si>
     <t>03.12.2021</t>
   </si>
   <si>
-    <t>15</t>
+    <t>717</t>
   </si>
   <si>
     <t>04.12.2021</t>
   </si>
   <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>18</t>
+    <t>715</t>
+  </si>
+  <si>
+    <t>705</t>
   </si>
 </sst>
 </file>
@@ -429,13 +438,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" customHeight="1">
@@ -443,7 +452,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14" customHeight="1">
@@ -451,7 +460,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14" customHeight="1">
@@ -511,7 +520,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14" customHeight="1">
@@ -519,10 +528,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14" customHeight="1">
@@ -530,10 +539,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14" customHeight="1">
@@ -541,7 +550,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14" customHeight="1">
@@ -549,7 +558,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14" customHeight="1">
@@ -582,7 +591,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14" customHeight="1">
@@ -590,7 +599,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14" customHeight="1">
@@ -598,7 +607,7 @@
         <v>22</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14" customHeight="1">
@@ -606,7 +615,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>